<commit_message>
Added computer vision results picture, will finish text after business
I just hit my head against a wall for 2 hours because of the fucking \headheight warning!!!!!!!!!
Updated size to 15
</commit_message>
<xml_diff>
--- a/0000_Docs/0004_Business/Risques.xlsx
+++ b/0000_Docs/0004_Business/Risques.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\LoRaSnow\0000_Docs\0004_Business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0230DFB-1E01-4938-8EA7-BF60BC519118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDC15F5-C3FC-428C-8CFC-5330FFB04269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3F60EF3E-183E-4FFD-B1B6-69BEADDE88BE}"/>
   </bookViews>
@@ -377,27 +377,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -405,23 +384,44 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,10 +737,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D648A5C-031B-4E6C-8347-C32FE732A0ED}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,25 +755,25 @@
     <row r="1" spans="1:13" ht="37.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
       <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="93.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -792,15 +795,20 @@
         <v>8</v>
       </c>
       <c r="H3" s="6"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="93.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="26" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="1"/>
@@ -808,16 +816,16 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="24" t="s">
+      <c r="I4" s="13"/>
+      <c r="J4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
     </row>
     <row r="5" spans="1:13" ht="93.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
@@ -825,77 +833,82 @@
       <c r="D5" s="7"/>
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="24" t="s">
+      <c r="I5" s="14"/>
+      <c r="J5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
     </row>
     <row r="6" spans="1:13" ht="93.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="12" t="s">
         <v>21</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="24" t="s">
+      <c r="I6" s="15"/>
+      <c r="J6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
     </row>
     <row r="7" spans="1:13" ht="93.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="18" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="1"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="24" t="s">
+      <c r="I7" s="16"/>
+      <c r="J7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
     </row>
     <row r="8" spans="1:13" ht="93.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="20" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="19" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
@@ -905,6 +918,11 @@
       <c r="F9" s="4"/>
       <c r="G9" s="6"/>
       <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -918,6 +936,6 @@
     <mergeCell ref="J6:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="67" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>